<commit_message>
Added information about fixing ART-DECOR issue
</commit_message>
<xml_diff>
--- a/src/main/resources/defaultiCRFSettings.xlsx
+++ b/src/main/resources/defaultiCRFSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\werk\projects\iCRFGenerator\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mine\projects\iCRFGenerator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF4BFCC-73F8-409F-8CA3-CD32B853CA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A79AE31-2228-4B41-9ECA-9F91014CDA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="645" windowWidth="26340" windowHeight="18060" activeTab="1" xr2:uid="{46BEC91F-C0CE-4829-B896-FA1B78700B4F}"/>
+    <workbookView xWindow="3165" yWindow="1500" windowWidth="20520" windowHeight="11775" activeTab="1" xr2:uid="{46BEC91F-C0CE-4829-B896-FA1B78700B4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -865,9 +865,6 @@
     <t>cbs-dstat-</t>
   </si>
   <si>
-    <t>https://decor.nictiz.nl/services/</t>
-  </si>
-  <si>
     <t>FAIRGenomes</t>
   </si>
   <si>
@@ -1106,6 +1103,9 @@
   </si>
   <si>
     <t>Basisgegevenssset Zorg 2020</t>
+  </si>
+  <si>
+    <t>https://decor.nictiz.nl/decor/services/</t>
   </si>
 </sst>
 </file>
@@ -1478,32 +1478,32 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1516,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,30 +1535,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" t="s">
         <v>301</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>302</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>303</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>304</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1" t="s">
         <v>305</v>
-      </c>
-      <c r="F1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B2" t="s">
         <v>271</v>
@@ -1567,38 +1567,38 @@
         <v>272</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" t="s">
         <v>355</v>
-      </c>
-      <c r="C3" t="s">
-        <v>354</v>
-      </c>
-      <c r="D3" t="s">
-        <v>275</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B4" t="s">
         <v>273</v>
@@ -1607,236 +1607,236 @@
         <v>274</v>
       </c>
       <c r="D4" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" t="s">
         <v>276</v>
       </c>
-      <c r="C5" t="s">
-        <v>277</v>
-      </c>
       <c r="D5" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" t="s">
         <v>278</v>
       </c>
-      <c r="C6" t="s">
-        <v>279</v>
-      </c>
       <c r="D6" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" t="s">
         <v>280</v>
       </c>
-      <c r="C7" t="s">
-        <v>281</v>
-      </c>
       <c r="D7" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" t="s">
         <v>282</v>
       </c>
-      <c r="C8" t="s">
-        <v>283</v>
-      </c>
       <c r="D8" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" t="s">
         <v>284</v>
       </c>
-      <c r="C9" t="s">
-        <v>285</v>
-      </c>
       <c r="D9" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" t="s">
         <v>287</v>
       </c>
-      <c r="C10" t="s">
-        <v>288</v>
-      </c>
       <c r="D10" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" t="s">
         <v>289</v>
       </c>
-      <c r="C11" t="s">
-        <v>290</v>
-      </c>
       <c r="D11" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B12" t="s">
+        <v>290</v>
+      </c>
+      <c r="C12" t="s">
         <v>291</v>
       </c>
-      <c r="C12" t="s">
-        <v>292</v>
-      </c>
       <c r="D12" t="s">
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="E12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B13" t="s">
         <v>293</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>294</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>295</v>
-      </c>
-      <c r="D13" t="s">
-        <v>296</v>
       </c>
       <c r="E13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C14" t="s">
         <v>297</v>
       </c>
-      <c r="C14" t="s">
-        <v>298</v>
-      </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B15" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" t="s">
         <v>299</v>
       </c>
-      <c r="C15" t="s">
-        <v>300</v>
-      </c>
       <c r="D15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -1966,7 +1966,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1988,7 +1988,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -2044,13 +2044,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B29" t="s">
         <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B48" t="s">
         <v>101</v>
       </c>
       <c r="C48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2814,13 +2814,13 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B73" t="s">
         <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,13 +2968,13 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B87" t="s">
         <v>175</v>
       </c>
       <c r="C87" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3133,13 +3133,13 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B102" t="s">
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3210,13 +3210,13 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B109" t="s">
         <v>213</v>
       </c>
       <c r="C109" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3254,13 +3254,13 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B113" t="s">
         <v>219</v>
       </c>
       <c r="C113" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3287,13 +3287,13 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B116" t="s">
         <v>223</v>
       </c>
       <c r="C116" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3375,13 +3375,13 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B124" t="s">
         <v>237</v>
       </c>
       <c r="C124" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3507,13 +3507,13 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B136" t="s">
         <v>259</v>
       </c>
       <c r="C136" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>